<commit_message>
Import from excel added
</commit_message>
<xml_diff>
--- a/data/groups.xlsx
+++ b/data/groups.xlsx
@@ -26,13 +26,13 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>name2L</t>
+    <t>test group</t>
   </si>
   <si>
-    <t xml:space="preserve">nameS </t>
+    <t>nameB</t>
   </si>
   <si>
-    <t>x</t>
+    <t>z</t>
   </si>
 </sst>
 </file>
@@ -354,24 +354,27 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="3" width="26" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>